<commit_message>
Changes to be committed: 	modified:   lens.xlsx
</commit_message>
<xml_diff>
--- a/lens.xlsx
+++ b/lens.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\scnsih\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\scnsih\Desktop\zleissca\lens\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BA70ADA4-2BB1-4AE1-83DF-758975A12F0E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BFBF552C-76D2-4CB6-AE97-15B737AC2DEE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{12EA1296-5616-4F8E-A678-CE4A2B6CF75D}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="21">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="26">
   <si>
     <t>15-35</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -74,10 +74,6 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>135L</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>京东</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -119,6 +115,25 @@
   </si>
   <si>
     <t>50 f1.2 G</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>r6</t>
+  </si>
+  <si>
+    <t>r62</t>
+  </si>
+  <si>
+    <t>r5</t>
+  </si>
+  <si>
+    <t>a7r3a</t>
+  </si>
+  <si>
+    <t>a73</t>
+  </si>
+  <si>
+    <t>starts</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -126,7 +141,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -144,10 +159,27 @@
     </font>
     <font>
       <b/>
-      <sz val="6"/>
+      <sz val="8"/>
       <color rgb="FFFF4400"/>
       <name val="Verdana"/>
       <family val="2"/>
+    </font>
+    <font>
+      <sz val="8"/>
+      <color theme="1"/>
+      <name val="等线"/>
+      <family val="2"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FF00B050"/>
+      <name val="等线"/>
+      <family val="3"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="2">
@@ -172,11 +204,17 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1">
       <alignment vertical="center"/>
     </xf>
   </cellXfs>
@@ -493,226 +531,314 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{74126D69-0E27-4ED4-A369-00ED007AA993}">
-  <dimension ref="A1:C24"/>
+  <dimension ref="A1:D31"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="F17" sqref="F17"/>
+      <selection activeCell="F15" sqref="F15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="10.58203125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="10.58203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
       <c r="B1" t="s">
+        <v>25</v>
+      </c>
+      <c r="C1" t="s">
+        <v>9</v>
+      </c>
+      <c r="D1" t="s">
         <v>10</v>
       </c>
-      <c r="C1" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>0</v>
       </c>
-      <c r="B2">
+      <c r="C2">
         <v>15499</v>
       </c>
-      <c r="C2" s="1">
+      <c r="D2" s="1">
         <v>11699</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>1</v>
       </c>
-      <c r="B3">
+      <c r="C3">
         <v>9999</v>
       </c>
-      <c r="C3" s="1">
+      <c r="D3" s="1">
         <v>8900</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>2</v>
       </c>
-      <c r="B4">
+      <c r="C4">
         <v>7588</v>
       </c>
-      <c r="C4" s="1">
+      <c r="D4" s="1">
         <v>6799</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>3</v>
       </c>
-      <c r="B5">
+      <c r="C5">
         <v>14499</v>
       </c>
-      <c r="C5" s="1">
+      <c r="D5" s="1">
         <v>13999</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
-        <v>12</v>
-      </c>
-      <c r="B6">
+        <v>11</v>
+      </c>
+      <c r="C6">
         <v>25699</v>
       </c>
-      <c r="C6" s="1">
+      <c r="D6" s="1">
         <v>21999</v>
       </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>4</v>
       </c>
-      <c r="B7">
+      <c r="C7">
         <v>11799</v>
       </c>
-      <c r="C7" s="1">
+      <c r="D7" s="1">
         <v>9299</v>
       </c>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>5</v>
       </c>
-      <c r="B8">
+      <c r="C8">
         <v>17699</v>
       </c>
-      <c r="C8" s="1">
+      <c r="D8" s="1">
         <v>15799</v>
       </c>
     </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>6</v>
       </c>
-      <c r="B9">
+      <c r="C9">
         <v>25999</v>
       </c>
-      <c r="C9" s="1">
+      <c r="D9" s="1">
         <v>18299</v>
       </c>
     </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="D10" s="2"/>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
         <v>7</v>
       </c>
-      <c r="B11">
-        <v>19999</v>
-      </c>
-      <c r="C11" s="1">
-        <v>16590</v>
-      </c>
-    </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="B11" s="3">
+        <v>4.5</v>
+      </c>
+      <c r="C11">
+        <v>20000</v>
+      </c>
+      <c r="D11" s="1">
+        <v>16600</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
         <v>8</v>
       </c>
-      <c r="B12">
-        <v>19899</v>
-      </c>
-    </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A13" t="s">
-        <v>9</v>
-      </c>
-      <c r="C13" s="1">
-        <v>18399</v>
-      </c>
-    </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="B12" s="3">
+        <v>4.75</v>
+      </c>
+      <c r="C12">
+        <v>19900</v>
+      </c>
+      <c r="D12" s="2"/>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="D13" s="1"/>
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="D14" s="2"/>
+    </row>
+    <row r="15" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
+        <v>12</v>
+      </c>
+      <c r="C15">
+        <v>4399</v>
+      </c>
+      <c r="D15" s="1">
+        <v>3499</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A16" t="s">
         <v>13</v>
       </c>
-      <c r="B15">
+      <c r="C16">
         <v>4399</v>
       </c>
-      <c r="C15" s="1">
-        <v>3499</v>
-      </c>
-    </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A16" t="s">
+      <c r="D16" s="1">
+        <v>3730</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A17" t="s">
         <v>14</v>
       </c>
-      <c r="B16">
-        <v>4399</v>
-      </c>
-      <c r="C16" s="1">
-        <v>3730</v>
-      </c>
-    </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A17" t="s">
+      <c r="C17">
+        <v>4299</v>
+      </c>
+      <c r="D17" s="1">
+        <v>3850</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="D18" s="1"/>
+    </row>
+    <row r="19" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A19" t="s">
+        <v>20</v>
+      </c>
+      <c r="C19">
+        <v>14000</v>
+      </c>
+      <c r="D19" s="1">
+        <v>13400</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A20" t="s">
+        <v>21</v>
+      </c>
+      <c r="C20">
+        <v>16500</v>
+      </c>
+      <c r="D20" s="1">
+        <v>16400</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A21" t="s">
+        <v>22</v>
+      </c>
+      <c r="C21">
+        <v>25600</v>
+      </c>
+      <c r="D21" s="1"/>
+    </row>
+    <row r="22" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="D22" s="2"/>
+    </row>
+    <row r="23" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="D23" s="2"/>
+    </row>
+    <row r="24" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A24" t="s">
         <v>15</v>
       </c>
-      <c r="B17">
-        <v>4299</v>
-      </c>
-      <c r="C17" s="1">
-        <v>3850</v>
-      </c>
-    </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A20" t="s">
+      <c r="B24" s="3">
+        <v>4</v>
+      </c>
+      <c r="C24">
+        <v>6900</v>
+      </c>
+      <c r="D24" s="1">
+        <v>6500</v>
+      </c>
+    </row>
+    <row r="25" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A25" t="s">
         <v>16</v>
       </c>
-      <c r="B20">
-        <v>6900</v>
-      </c>
-      <c r="C20" s="1">
-        <v>6500</v>
-      </c>
-    </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A21" t="s">
+      <c r="B25" s="3">
+        <v>4</v>
+      </c>
+      <c r="C25">
+        <v>10200</v>
+      </c>
+      <c r="D25" s="1">
+        <v>9250</v>
+      </c>
+    </row>
+    <row r="26" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A26" t="s">
         <v>17</v>
       </c>
-      <c r="B21">
-        <v>10200</v>
-      </c>
-      <c r="C21" s="1">
-        <v>9250</v>
-      </c>
-    </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A22" t="s">
+      <c r="B26" s="3"/>
+      <c r="C26">
+        <v>10500</v>
+      </c>
+      <c r="D26" s="1">
+        <v>8200</v>
+      </c>
+    </row>
+    <row r="27" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A27" t="s">
+        <v>19</v>
+      </c>
+      <c r="B27" s="3"/>
+      <c r="C27">
+        <v>15300</v>
+      </c>
+      <c r="D27" s="1">
+        <v>12300</v>
+      </c>
+    </row>
+    <row r="28" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A28" t="s">
         <v>18</v>
       </c>
-      <c r="B22">
+      <c r="B28" s="3">
+        <v>4.25</v>
+      </c>
+      <c r="C28">
         <v>10500</v>
       </c>
-      <c r="C22" s="1">
-        <v>8199</v>
-      </c>
-    </row>
-    <row r="23" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A23" t="s">
-        <v>20</v>
-      </c>
-      <c r="B23">
-        <v>15300</v>
-      </c>
-      <c r="C23" s="1">
-        <v>12299</v>
-      </c>
-    </row>
-    <row r="24" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A24" t="s">
-        <v>19</v>
-      </c>
-      <c r="B24">
+      <c r="D28" s="1">
+        <v>9700</v>
+      </c>
+    </row>
+    <row r="29" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="D29" s="2"/>
+    </row>
+    <row r="30" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A30" t="s">
+        <v>23</v>
+      </c>
+      <c r="C30">
+        <v>14500</v>
+      </c>
+      <c r="D30" s="1">
+        <v>14000</v>
+      </c>
+    </row>
+    <row r="31" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A31" t="s">
+        <v>24</v>
+      </c>
+      <c r="C31">
+        <v>11000</v>
+      </c>
+      <c r="D31" s="1">
         <v>10500</v>
-      </c>
-      <c r="C24" s="1">
-        <v>9700</v>
       </c>
     </row>
   </sheetData>

</xml_diff>